<commit_message>
Attempting to fix json file export error
</commit_message>
<xml_diff>
--- a/Documentation/tests/userEvaluationResults.xlsx
+++ b/Documentation/tests/userEvaluationResults.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="30">
   <si>
     <t>Participant</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Sums</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;- Joe </t>
   </si>
 </sst>
 </file>
@@ -206,15 +203,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,17 +237,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -263,14 +255,22 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
     <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="4" builtinId="39"/>
     <cellStyle name="40% - Accent4" xfId="5" builtinId="43"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -362,7 +362,7 @@
                   <c:v>34.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.428571428571427</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>35</c:v>
@@ -430,7 +430,7 @@
                   <c:v>21.666666666666668</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.571428571428571</c:v>
+                  <c:v>11.625</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>18</c:v>
@@ -498,7 +498,7 @@
                   <c:v>10.666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>10</c:v>
@@ -516,11 +516,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="132591104"/>
-        <c:axId val="122606656"/>
+        <c:axId val="78786048"/>
+        <c:axId val="121885760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="132591104"/>
+        <c:axId val="78786048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,7 +530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122606656"/>
+        <c:crossAx val="121885760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -538,7 +538,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122606656"/>
+        <c:axId val="121885760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +549,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132591104"/>
+        <c:crossAx val="78786048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -784,7 +784,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1040,7 +1040,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7</c:v>
@@ -1464,7 +1464,7 @@
   <dimension ref="A1:Y46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X28" sqref="X28"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,16 +1608,16 @@
       <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="U5" s="10" t="s">
+      <c r="U5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="V5" s="10">
+      <c r="V5" s="12">
         <v>21</v>
       </c>
-      <c r="W5" s="10">
+      <c r="W5" s="12">
         <v>12</v>
       </c>
-      <c r="X5" s="10">
+      <c r="X5" s="12">
         <v>8</v>
       </c>
       <c r="Y5">
@@ -1650,16 +1650,16 @@
       <c r="H6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="U6" s="10" t="s">
+      <c r="U6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="V6" s="10">
+      <c r="V6" s="12">
         <v>35</v>
       </c>
-      <c r="W6" s="10">
+      <c r="W6" s="12">
         <v>13</v>
       </c>
-      <c r="X6" s="10">
+      <c r="X6" s="12">
         <v>9</v>
       </c>
       <c r="Y6">
@@ -1692,16 +1692,16 @@
       <c r="H7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="U7" s="10" t="s">
+      <c r="U7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="V7" s="10">
+      <c r="V7" s="12">
         <v>14</v>
       </c>
-      <c r="W7" s="10">
+      <c r="W7" s="12">
         <v>11</v>
       </c>
-      <c r="X7" s="10">
+      <c r="X7" s="12">
         <v>4</v>
       </c>
       <c r="Y7">
@@ -1734,7 +1734,7 @@
       <c r="H8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="U8" s="10" t="s">
+      <c r="U8" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1757,7 +1757,7 @@
       <c r="F9" s="3">
         <v>9</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="13" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -1783,13 +1783,13 @@
       <c r="F10" s="3">
         <v>8</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="13" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="U10" s="10" t="s">
+      <c r="U10" s="12" t="s">
         <v>28</v>
       </c>
       <c r="V10">
@@ -1797,11 +1797,11 @@
         <v>23.333333333333332</v>
       </c>
       <c r="W10">
-        <f t="shared" ref="W10:X10" si="1">AVERAGE(W5:W7)</f>
+        <f>AVERAGE(W5:W7)</f>
         <v>12</v>
       </c>
       <c r="X10">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(X5:X7)</f>
         <v>7</v>
       </c>
       <c r="Y10">
@@ -2001,13 +2001,20 @@
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" t="s">
-        <v>30</v>
+      <c r="D18" s="15">
+        <v>28</v>
+      </c>
+      <c r="E18" s="15">
+        <v>12</v>
+      </c>
+      <c r="F18" s="15">
+        <v>6</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2029,7 +2036,7 @@
       <c r="F19" s="1">
         <v>6</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -2081,11 +2088,11 @@
       <c r="F21" s="1">
         <v>6</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>10</v>
+      <c r="G21" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2170,34 +2177,34 @@
       <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D27" s="8">
         <f>AVERAGE(D2:D24)</f>
-        <v>35.545454545454547</v>
+        <v>35.217391304347828</v>
       </c>
       <c r="E27" s="8">
-        <f t="shared" ref="E27:F27" si="2">AVERAGE(E2:E24)</f>
-        <v>18.5</v>
+        <f t="shared" ref="E27:F27" si="1">AVERAGE(E2:E24)</f>
+        <v>18.217391304347824</v>
       </c>
       <c r="F27" s="8">
-        <f t="shared" si="2"/>
-        <v>10.409090909090908</v>
+        <f t="shared" si="1"/>
+        <v>10.217391304347826</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
@@ -2221,23 +2228,23 @@
       <c r="C31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="10">
         <f>AVERAGE(D2:D8)</f>
         <v>57</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="10">
         <f>AVERAGE(D9:D13)</f>
         <v>28.8</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F31" s="10">
         <f>AVERAGE(D14:D16)</f>
         <v>34.333333333333336</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="10">
         <f>AVERAGE(D17:D24)</f>
-        <v>19.428571428571427</v>
-      </c>
-      <c r="H31" s="11">
+        <v>20.5</v>
+      </c>
+      <c r="H31" s="10">
         <v>35</v>
       </c>
     </row>
@@ -2245,23 +2252,23 @@
       <c r="C32" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="10">
         <f>AVERAGE(E2:E8)</f>
         <v>27.714285714285715</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="10">
         <f>AVERAGE(E9:E13)</f>
         <v>13.4</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="10">
         <f>AVERAGE(E14:E16)</f>
         <v>21.666666666666668</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="10">
         <f>AVERAGE(E17:E24)</f>
-        <v>11.571428571428571</v>
-      </c>
-      <c r="H32" s="11">
+        <v>11.625</v>
+      </c>
+      <c r="H32" s="10">
         <v>18</v>
       </c>
     </row>
@@ -2269,123 +2276,135 @@
       <c r="C33" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="10">
         <f>AVERAGE(F2:F8)</f>
         <v>16.285714285714285</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="10">
         <f>AVERAGE(F9:F13)</f>
         <v>9.6</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F33" s="10">
         <f>AVERAGE(F14:F16)</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="10">
         <f>AVERAGE(F17:F24)</f>
-        <v>5</v>
-      </c>
-      <c r="H33" s="11">
+        <v>5.125</v>
+      </c>
+      <c r="H33" s="10">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C34" s="9"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C35" s="9"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C37" s="12"/>
-      <c r="D37" s="12" t="s">
+      <c r="C37" s="11"/>
+      <c r="D37" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F37" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G37" s="12" t="s">
+      <c r="G37" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="12">
+      <c r="D38" s="11">
         <f>COUNTIF($G$2:$G$8,"=OF")</f>
         <v>5</v>
       </c>
-      <c r="E38" s="12">
+      <c r="E38" s="11">
         <f>COUNTIF($G$9:$G$13,"=OF")</f>
         <v>3</v>
       </c>
-      <c r="F38" s="12">
+      <c r="F38" s="11">
         <f>COUNTIF($G$14:$G$16,"=OF")</f>
         <v>2</v>
       </c>
-      <c r="G38" s="12">
+      <c r="G38" s="11">
         <f>COUNTIF(G$17:$G$24,"=OF")</f>
         <v>5</v>
       </c>
+      <c r="H38" s="18">
+        <f>SUM(D38:G38)/A24</f>
+        <v>0.65217391304347827</v>
+      </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D39" s="12">
+      <c r="D39" s="11">
         <f>COUNTIF($G$2:$G$8,"=M")</f>
         <v>2</v>
       </c>
-      <c r="E39" s="12">
+      <c r="E39" s="11">
         <f>COUNTIF($G$9:$G$13,"=M")</f>
         <v>2</v>
       </c>
-      <c r="F39" s="12">
+      <c r="F39" s="11">
         <f>COUNTIF($G$14:$G$16,"=M")</f>
         <v>1</v>
       </c>
-      <c r="G39" s="12">
+      <c r="G39" s="11">
         <f>COUNTIF(G$17:$G$24,"=M")</f>
         <v>2</v>
       </c>
+      <c r="H39" s="18">
+        <f>SUM(D39:G39)/A24</f>
+        <v>0.30434782608695654</v>
+      </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="12">
+      <c r="D40" s="11">
         <f>COUNTIF($G$2:$G$8,"=FTU")</f>
         <v>0</v>
       </c>
-      <c r="E40" s="12">
+      <c r="E40" s="11">
         <f>COUNTIF($G$9:$G$13,"=FTU")</f>
         <v>0</v>
       </c>
-      <c r="F40" s="12">
+      <c r="F40" s="11">
         <f>COUNTIF($G$14:$G$16,"=FTU")</f>
         <v>0</v>
       </c>
-      <c r="G40" s="12">
+      <c r="G40" s="11">
         <f>COUNTIF(G$17:$G$24,"=FTU")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H40" s="18">
+        <f>SUM(D40:G40)/A24</f>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
@@ -2394,90 +2413,102 @@
       <c r="F41" s="9"/>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C43" s="12"/>
-      <c r="D43" s="12" t="s">
+      <c r="C43" s="11"/>
+      <c r="D43" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="12" t="s">
+      <c r="F43" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G43" s="12" t="s">
+      <c r="G43" s="11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="12">
+      <c r="D44" s="11">
         <f>COUNTIF($H$2:$H$8,"=OF")</f>
         <v>0</v>
       </c>
-      <c r="E44" s="12">
+      <c r="E44" s="11">
         <f>COUNTIF($H$9:$H$13,"=OF")</f>
         <v>0</v>
       </c>
-      <c r="F44" s="12">
+      <c r="F44" s="11">
         <f>COUNTIF($H$14:$H$16,"=OF")</f>
         <v>0</v>
       </c>
-      <c r="G44" s="12">
+      <c r="G44" s="11">
         <f>COUNTIF(H$17:$H$24,"=OF")</f>
         <v>0</v>
       </c>
+      <c r="H44" s="18">
+        <f>SUM(D44:G44)/A24</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D45" s="12">
+      <c r="D45" s="11">
         <f>COUNTIF($H$2:$H$8,"=M")</f>
         <v>0</v>
       </c>
-      <c r="E45" s="12">
+      <c r="E45" s="11">
         <f>COUNTIF($H$9:$H$13,"=M")</f>
         <v>0</v>
       </c>
-      <c r="F45" s="12">
+      <c r="F45" s="11">
         <f>COUNTIF($H$14:HG$16,"=M")</f>
         <v>0</v>
       </c>
-      <c r="G45" s="12">
+      <c r="G45" s="11">
         <f>COUNTIF(H$17:$H$24,"=M")</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H45" s="18">
+        <f>SUM(D45:G45)/A24</f>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D46" s="12">
+      <c r="D46" s="11">
         <f>COUNTIF($H$2:$H$8,"=FTU")</f>
         <v>7</v>
       </c>
-      <c r="E46" s="12">
+      <c r="E46" s="11">
         <f>COUNTIF($H$9:$H$13,"=FTU")</f>
         <v>5</v>
       </c>
-      <c r="F46" s="12">
+      <c r="F46" s="11">
         <f>COUNTIF($H$14:$H$16,"=FTU")</f>
         <v>3</v>
       </c>
-      <c r="G46" s="12">
+      <c r="G46" s="11">
         <f>COUNTIF(H$17:$H$24,"=FTU")</f>
         <v>7</v>
+      </c>
+      <c r="H46" s="18">
+        <f>SUM(D46:G46)/A24</f>
+        <v>0.95652173913043481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added results of user evaluation into appendix, begun evaluation section
</commit_message>
<xml_diff>
--- a/Documentation/tests/userEvaluationResults.xlsx
+++ b/Documentation/tests/userEvaluationResults.xlsx
@@ -16,17 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="28">
   <si>
     <t>Participant</t>
   </si>
   <si>
-    <t>Fuzzy Skill</t>
-  </si>
-  <si>
-    <t>Comp Skill</t>
-  </si>
-  <si>
     <t>Task 1</t>
   </si>
   <si>
@@ -42,9 +36,6 @@
     <t>Least Liked</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
     <t>OF</t>
   </si>
   <si>
@@ -54,12 +45,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High </t>
-  </si>
-  <si>
     <t>Averages</t>
   </si>
   <si>
@@ -106,6 +91,15 @@
   </si>
   <si>
     <t>Sums</t>
+  </si>
+  <si>
+    <t>Most Liked Software</t>
+  </si>
+  <si>
+    <t>Least Liked Software</t>
+  </si>
+  <si>
+    <t>Group</t>
   </si>
 </sst>
 </file>
@@ -179,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -202,6 +196,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -212,7 +241,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -255,13 +284,34 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -516,11 +566,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="78786048"/>
-        <c:axId val="121885760"/>
+        <c:axId val="133053952"/>
+        <c:axId val="124048448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78786048"/>
+        <c:axId val="133053952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,7 +580,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121885760"/>
+        <c:crossAx val="124048448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -538,7 +588,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121885760"/>
+        <c:axId val="124048448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +599,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78786048"/>
+        <c:crossAx val="133053952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1464,14 +1514,13 @@
   <dimension ref="A1:Y46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="AA23" sqref="AA23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1480,38 +1529,34 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B2" s="22">
+        <v>1</v>
+      </c>
+      <c r="C2" s="22"/>
       <c r="D2" s="4">
         <v>53</v>
       </c>
@@ -1522,22 +1567,20 @@
         <v>14</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B3" s="21">
+        <v>1</v>
+      </c>
+      <c r="C3" s="21"/>
       <c r="D3" s="4">
         <v>45</v>
       </c>
@@ -1548,22 +1591,20 @@
         <v>15</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B4" s="21">
+        <v>1</v>
+      </c>
+      <c r="C4" s="21"/>
       <c r="D4" s="4">
         <v>61</v>
       </c>
@@ -1574,25 +1615,23 @@
         <v>20</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Y4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B5" s="21">
+        <v>1</v>
+      </c>
+      <c r="C5" s="21"/>
       <c r="D5" s="4">
         <v>70</v>
       </c>
@@ -1603,13 +1642,13 @@
         <v>21</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="V5" s="12">
         <v>21</v>
@@ -1629,12 +1668,10 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B6" s="21">
+        <v>1</v>
+      </c>
+      <c r="C6" s="21"/>
       <c r="D6" s="4">
         <v>63</v>
       </c>
@@ -1645,13 +1682,13 @@
         <v>15</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="V6" s="12">
         <v>35</v>
@@ -1671,12 +1708,10 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B7" s="21">
+        <v>1</v>
+      </c>
+      <c r="C7" s="21"/>
       <c r="D7" s="4">
         <v>53</v>
       </c>
@@ -1687,13 +1722,13 @@
         <v>13</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="V7" s="12">
         <v>14</v>
@@ -1713,12 +1748,10 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B8" s="21">
+        <v>1</v>
+      </c>
+      <c r="C8" s="21"/>
       <c r="D8" s="4">
         <v>54</v>
       </c>
@@ -1729,25 +1762,23 @@
         <v>16</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="B9" s="23">
+        <v>2</v>
+      </c>
+      <c r="C9" s="23"/>
       <c r="D9" s="3">
         <v>35</v>
       </c>
@@ -1758,22 +1789,20 @@
         <v>9</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="B10" s="23">
+        <v>2</v>
+      </c>
+      <c r="C10" s="23"/>
       <c r="D10" s="3">
         <v>25</v>
       </c>
@@ -1784,13 +1813,13 @@
         <v>8</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="U10" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="V10">
         <f>AVERAGE(V5:V7)</f>
@@ -1813,12 +1842,10 @@
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="B11" s="23">
+        <v>2</v>
+      </c>
+      <c r="C11" s="23"/>
       <c r="D11" s="3">
         <v>27</v>
       </c>
@@ -1829,22 +1856,20 @@
         <v>10</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="B12" s="23">
+        <v>2</v>
+      </c>
+      <c r="C12" s="23"/>
       <c r="D12" s="3">
         <v>26</v>
       </c>
@@ -1855,22 +1880,20 @@
         <v>11</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="B13" s="23">
+        <v>2</v>
+      </c>
+      <c r="C13" s="23"/>
       <c r="D13" s="3">
         <v>31</v>
       </c>
@@ -1881,22 +1904,20 @@
         <v>10</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="B14" s="24">
+        <v>3</v>
+      </c>
+      <c r="C14" s="24"/>
       <c r="D14" s="2">
         <v>33</v>
       </c>
@@ -1907,22 +1928,20 @@
         <v>9</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="B15" s="24">
+        <v>3</v>
+      </c>
+      <c r="C15" s="24"/>
       <c r="D15" s="2">
         <v>30</v>
       </c>
@@ -1933,22 +1952,20 @@
         <v>10</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="B16" s="24">
+        <v>3</v>
+      </c>
+      <c r="C16" s="24"/>
       <c r="D16" s="2">
         <v>40</v>
       </c>
@@ -1959,22 +1976,20 @@
         <v>13</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B17" s="25">
+        <v>4</v>
+      </c>
+      <c r="C17" s="25"/>
       <c r="D17" s="1">
         <v>14</v>
       </c>
@@ -1985,22 +2000,20 @@
         <v>4</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B18" s="25">
+        <v>4</v>
+      </c>
+      <c r="C18" s="25"/>
       <c r="D18" s="15">
         <v>28</v>
       </c>
@@ -2011,22 +2024,20 @@
         <v>6</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B19" s="25">
+        <v>4</v>
+      </c>
+      <c r="C19" s="25"/>
       <c r="D19" s="1">
         <v>20</v>
       </c>
@@ -2037,22 +2048,20 @@
         <v>6</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B20" s="25">
+        <v>4</v>
+      </c>
+      <c r="C20" s="25"/>
       <c r="D20" s="1">
         <v>21</v>
       </c>
@@ -2063,22 +2072,20 @@
         <v>5</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B21" s="25">
+        <v>4</v>
+      </c>
+      <c r="C21" s="25"/>
       <c r="D21" s="1">
         <v>22</v>
       </c>
@@ -2089,22 +2096,20 @@
         <v>6</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B22" s="25">
+        <v>4</v>
+      </c>
+      <c r="C22" s="25"/>
       <c r="D22" s="1">
         <v>25</v>
       </c>
@@ -2115,22 +2120,20 @@
         <v>4</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B23" s="25">
+        <v>4</v>
+      </c>
+      <c r="C23" s="25"/>
       <c r="D23" s="1">
         <v>18</v>
       </c>
@@ -2141,22 +2144,20 @@
         <v>5</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B24" s="25">
+        <v>4</v>
+      </c>
+      <c r="C24" s="25"/>
       <c r="D24" s="1">
         <v>16</v>
       </c>
@@ -2167,21 +2168,21 @@
         <v>5</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D26" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
+      <c r="D26" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D27" s="8">
@@ -2198,35 +2199,35 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C29" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
+      <c r="C29" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
       <c r="D30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C31" s="9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D31" s="10">
         <f>AVERAGE(D2:D8)</f>
@@ -2250,7 +2251,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C32" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D32" s="10">
         <f>AVERAGE(E2:E8)</f>
@@ -2274,7 +2275,7 @@
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C33" s="9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D33" s="10">
         <f>AVERAGE(F2:F8)</f>
@@ -2309,32 +2310,32 @@
       <c r="F35" s="10"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C36" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
+      <c r="C36" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C37" s="11"/>
       <c r="D37" s="11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C38" s="11" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D38" s="11">
         <f>COUNTIF($G$2:$G$8,"=OF")</f>
@@ -2352,14 +2353,14 @@
         <f>COUNTIF(G$17:$G$24,"=OF")</f>
         <v>5</v>
       </c>
-      <c r="H38" s="18">
+      <c r="H38" s="16">
         <f>SUM(D38:G38)/A24</f>
         <v>0.65217391304347827</v>
       </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C39" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D39" s="11">
         <f>COUNTIF($G$2:$G$8,"=M")</f>
@@ -2377,14 +2378,14 @@
         <f>COUNTIF(G$17:$G$24,"=M")</f>
         <v>2</v>
       </c>
-      <c r="H39" s="18">
+      <c r="H39" s="16">
         <f>SUM(D39:G39)/A24</f>
         <v>0.30434782608695654</v>
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C40" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D40" s="11">
         <f>COUNTIF($G$2:$G$8,"=FTU")</f>
@@ -2402,7 +2403,7 @@
         <f>COUNTIF(G$17:$G$24,"=FTU")</f>
         <v>1</v>
       </c>
-      <c r="H40" s="18">
+      <c r="H40" s="16">
         <f>SUM(D40:G40)/A24</f>
         <v>4.3478260869565216E-2</v>
       </c>
@@ -2413,32 +2414,32 @@
       <c r="F41" s="9"/>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C42" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
+      <c r="C42" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C44" s="11" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D44" s="11">
         <f>COUNTIF($H$2:$H$8,"=OF")</f>
@@ -2456,14 +2457,14 @@
         <f>COUNTIF(H$17:$H$24,"=OF")</f>
         <v>0</v>
       </c>
-      <c r="H44" s="18">
+      <c r="H44" s="16">
         <f>SUM(D44:G44)/A24</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C45" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D45" s="11">
         <f>COUNTIF($H$2:$H$8,"=M")</f>
@@ -2481,14 +2482,14 @@
         <f>COUNTIF(H$17:$H$24,"=M")</f>
         <v>1</v>
       </c>
-      <c r="H45" s="18">
+      <c r="H45" s="16">
         <f>SUM(D45:G45)/A24</f>
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C46" s="11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D46" s="11">
         <f>COUNTIF($H$2:$H$8,"=FTU")</f>
@@ -2506,17 +2507,41 @@
         <f>COUNTIF(H$17:$H$24,"=FTU")</f>
         <v>7</v>
       </c>
-      <c r="H46" s="18">
+      <c r="H46" s="16">
         <f>SUM(D46:G46)/A24</f>
         <v>0.95652173913043481</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="28">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C42:G42"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C29:G29"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
table of participants and point of study included
</commit_message>
<xml_diff>
--- a/Documentation/tests/userEvaluationResults.xlsx
+++ b/Documentation/tests/userEvaluationResults.xlsx
@@ -638,53 +638,62 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:doughnutChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$36:$D$37</c:f>
+              <c:f>Sheet1!$C$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Most Liked Group 1</c:v>
+                  <c:v>O-Fuzz</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$38:$C$40</c:f>
+              <c:f>Sheet1!$D$37:$G$37</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>O-Fuzz</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Group 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>MATLAB</c:v>
+                  <c:v>Group 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>FuzzyToolkitUoN</c:v>
+                  <c:v>Group 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Group 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$38:$D$40</c:f>
+              <c:f>Sheet1!$D$38:$G$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -695,46 +704,53 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$36:$E$37</c:f>
+              <c:f>Sheet1!$C$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Most Liked Group 2</c:v>
+                  <c:v>MATLAB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$38:$C$40</c:f>
+              <c:f>Sheet1!$D$37:$G$37</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>O-Fuzz</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Group 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>MATLAB</c:v>
+                  <c:v>Group 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>FuzzyToolkitUoN</c:v>
+                  <c:v>Group 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Group 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$38:$E$40</c:f>
+              <c:f>Sheet1!$D$39:$G$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -745,95 +761,52 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$36:$F$37</c:f>
+              <c:f>Sheet1!$C$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Most Liked Group 3</c:v>
+                  <c:v>FuzzyToolkitUoN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$38:$C$40</c:f>
+              <c:f>Sheet1!$D$37:$G$37</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>O-Fuzz</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Group 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>MATLAB</c:v>
+                  <c:v>Group 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>FuzzyToolkitUoN</c:v>
+                  <c:v>Group 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Group 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$38:$F$40</c:f>
+              <c:f>Sheet1!$D$40:$G$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$G$36:$G$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Most Liked Group 4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$38:$C$40</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>O-Fuzz</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>MATLAB</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>FuzzyToolkitUoN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$38:$G$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -847,26 +820,50 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-        <c:holeSize val="50"/>
-      </c:doughnutChart>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="48471552"/>
+        <c:axId val="48531712"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="48471552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48531712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="48531712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48471552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -897,45 +894,51 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:doughnutChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$43</c:f>
+              <c:f>Sheet1!$C$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Group 1</c:v>
+                  <c:v>O-Fuzz</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$44:$C$46</c:f>
+              <c:f>Sheet1!$D$43:$G$43</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>O-Fuzz</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Group 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>MATLAB</c:v>
+                  <c:v>Group 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>FuzzyToolkitUoN</c:v>
+                  <c:v>Group 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Group 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$44:$D$46</c:f>
+              <c:f>Sheet1!$D$44:$G$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -943,7 +946,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -954,38 +960,42 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$43</c:f>
+              <c:f>Sheet1!$C$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Group 2</c:v>
+                  <c:v>MATLAB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$44:$C$46</c:f>
+              <c:f>Sheet1!$D$43:$G$43</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>O-Fuzz</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Group 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>MATLAB</c:v>
+                  <c:v>Group 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>FuzzyToolkitUoN</c:v>
+                  <c:v>Group 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Group 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$44:$E$46</c:f>
+              <c:f>Sheet1!$D$45:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -993,7 +1003,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1004,95 +1017,52 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$43</c:f>
+              <c:f>Sheet1!$C$46</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Group 3</c:v>
+                  <c:v>FuzzyToolkitUoN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$44:$C$46</c:f>
+              <c:f>Sheet1!$D$43:$G$43</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>O-Fuzz</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Group 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>MATLAB</c:v>
+                  <c:v>Group 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>FuzzyToolkitUoN</c:v>
+                  <c:v>Group 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Group 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$44:$F$46</c:f>
+              <c:f>Sheet1!$D$46:$G$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$G$43</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Group 4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$44:$C$46</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>O-Fuzz</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>MATLAB</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>FuzzyToolkitUoN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$44:$G$46</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
@@ -1106,11 +1076,45 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-        <c:holeSize val="50"/>
-      </c:doughnutChart>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="48467968"/>
+        <c:axId val="48534592"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="48467968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48534592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="48534592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48467968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -1164,19 +1168,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:colOff>233362</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1194,19 +1198,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:colOff>528637</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:colOff>223837</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1514,7 +1518,7 @@
   <dimension ref="A1:Y46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA23" sqref="AA23"/>
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,10 +2357,7 @@
         <f>COUNTIF(G$17:$G$24,"=OF")</f>
         <v>5</v>
       </c>
-      <c r="H38" s="16">
-        <f>SUM(D38:G38)/A24</f>
-        <v>0.65217391304347827</v>
-      </c>
+      <c r="H38" s="16"/>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C39" s="11" t="s">
@@ -2378,10 +2379,7 @@
         <f>COUNTIF(G$17:$G$24,"=M")</f>
         <v>2</v>
       </c>
-      <c r="H39" s="16">
-        <f>SUM(D39:G39)/A24</f>
-        <v>0.30434782608695654</v>
-      </c>
+      <c r="H39" s="16"/>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C40" s="11" t="s">
@@ -2403,10 +2401,7 @@
         <f>COUNTIF(G$17:$G$24,"=FTU")</f>
         <v>1</v>
       </c>
-      <c r="H40" s="16">
-        <f>SUM(D40:G40)/A24</f>
-        <v>4.3478260869565216E-2</v>
-      </c>
+      <c r="H40" s="16"/>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D41" s="9"/>
@@ -2457,10 +2452,7 @@
         <f>COUNTIF(H$17:$H$24,"=OF")</f>
         <v>0</v>
       </c>
-      <c r="H44" s="16">
-        <f>SUM(D44:G44)/A24</f>
-        <v>0</v>
-      </c>
+      <c r="H44" s="16"/>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C45" s="11" t="s">
@@ -2482,10 +2474,7 @@
         <f>COUNTIF(H$17:$H$24,"=M")</f>
         <v>1</v>
       </c>
-      <c r="H45" s="16">
-        <f>SUM(D45:G45)/A24</f>
-        <v>4.3478260869565216E-2</v>
-      </c>
+      <c r="H45" s="16"/>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C46" s="11" t="s">
@@ -2507,10 +2496,7 @@
         <f>COUNTIF(H$17:$H$24,"=FTU")</f>
         <v>7</v>
       </c>
-      <c r="H46" s="16">
-        <f>SUM(D46:G46)/A24</f>
-        <v>0.95652173913043481</v>
-      </c>
+      <c r="H46" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="28">

</xml_diff>

<commit_message>
Added a bunch of comments for the evaluation section, need to actually write it though...
</commit_message>
<xml_diff>
--- a/Documentation/tests/userEvaluationResults.xlsx
+++ b/Documentation/tests/userEvaluationResults.xlsx
@@ -285,6 +285,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -297,19 +306,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -346,6 +346,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Time taken to complete instruction</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> set in each software system, by group</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -362,7 +386,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Task 1</c:v>
+                  <c:v>FuzzyToolkitUoN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -412,7 +436,7 @@
                   <c:v>34.333333333333336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.5</c:v>
+                  <c:v>19.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>35</c:v>
@@ -430,7 +454,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Task 2</c:v>
+                  <c:v>MATLAB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -498,7 +522,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Task 3</c:v>
+                  <c:v>O-Fuzz</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -566,11 +590,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="133053952"/>
-        <c:axId val="124048448"/>
+        <c:axId val="91222016"/>
+        <c:axId val="67097664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133053952"/>
+        <c:axId val="91222016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -580,7 +604,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124048448"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="67097664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -588,18 +622,47 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124048448"/>
+        <c:axId val="67097664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800"/>
+                  <a:t>Time taken to complete tasks, in Minutes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133053952"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91222016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -608,6 +671,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -635,6 +708,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="2000"/>
+              <a:t>Least favourite piece</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="2000" baseline="0"/>
+              <a:t> of software by group, as a percentage</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="2000"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -647,7 +744,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$38</c:f>
+              <c:f>Sheet1!$C$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -659,7 +756,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$37:$G$37</c:f>
+              <c:f>Sheet1!$D$43:$G$43</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -679,21 +776,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$38:$G$38</c:f>
+              <c:f>Sheet1!$D$44:$G$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -704,7 +801,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$39</c:f>
+              <c:f>Sheet1!$C$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -716,7 +813,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$37:$G$37</c:f>
+              <c:f>Sheet1!$D$43:$G$43</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -736,21 +833,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$39:$G$39</c:f>
+              <c:f>Sheet1!$D$45:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -761,7 +858,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$40</c:f>
+              <c:f>Sheet1!$C$46</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -773,7 +870,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$37:$G$37</c:f>
+              <c:f>Sheet1!$D$43:$G$43</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -793,21 +890,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$40:$G$40</c:f>
+              <c:f>Sheet1!$D$46:$G$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -823,11 +920,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="48471552"/>
-        <c:axId val="48531712"/>
+        <c:axId val="91223552"/>
+        <c:axId val="67099968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48471552"/>
+        <c:axId val="91223552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -836,7 +933,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48531712"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="67099968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -844,18 +951,47 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48531712"/>
+        <c:axId val="67099968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800"/>
+                  <a:t>Percentage of particpants</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48471552"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91223552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -864,6 +1000,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -891,6 +1037,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="2000"/>
+              <a:t>Most favourite piece</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="2000" baseline="0"/>
+              <a:t> of software by group, as a percentage</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="2000"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -903,7 +1073,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$44</c:f>
+              <c:f>Sheet1!$C$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -915,7 +1085,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$43:$G$43</c:f>
+              <c:f>Sheet1!$D$37:$G$37</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -935,21 +1105,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$44:$G$44</c:f>
+              <c:f>Sheet1!$D$38:$G$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -960,7 +1130,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$45</c:f>
+              <c:f>Sheet1!$C$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -972,7 +1142,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$43:$G$43</c:f>
+              <c:f>Sheet1!$D$37:$G$37</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -992,21 +1162,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$45:$G$45</c:f>
+              <c:f>Sheet1!$D$39:$G$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1017,7 +1187,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$46</c:f>
+              <c:f>Sheet1!$C$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1029,7 +1199,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$D$43:$G$43</c:f>
+              <c:f>Sheet1!$D$37:$G$37</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1049,21 +1219,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$46:$G$46</c:f>
+              <c:f>Sheet1!$D$40:$G$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1079,11 +1249,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="48467968"/>
-        <c:axId val="48534592"/>
+        <c:axId val="91224064"/>
+        <c:axId val="132531904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48467968"/>
+        <c:axId val="91224064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1092,7 +1262,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48534592"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="132531904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1100,18 +1280,47 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48534592"/>
+        <c:axId val="132531904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800"/>
+                  <a:t>Percentage of particpants</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48467968"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="91224064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1120,6 +1329,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1138,15 +1357,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>138111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1167,20 +1386,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>538162</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>147636</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>233362</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1197,21 +1416,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>528637</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>223837</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>414338</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>157163</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1517,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,10 +1754,10 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="20"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1557,10 +1778,10 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="24">
         <v>1</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="4">
         <v>53</v>
       </c>
@@ -1581,10 +1802,10 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="25">
         <v>1</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="4">
         <v>45</v>
       </c>
@@ -1605,10 +1826,10 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="25">
         <v>1</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="4">
         <v>61</v>
       </c>
@@ -1632,10 +1853,10 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="25">
         <v>1</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="4">
         <v>70</v>
       </c>
@@ -1672,10 +1893,10 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="25">
         <v>1</v>
       </c>
-      <c r="C6" s="21"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="4">
         <v>63</v>
       </c>
@@ -1712,10 +1933,10 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="25">
         <v>1</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="4">
         <v>53</v>
       </c>
@@ -1752,10 +1973,10 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="25">
         <v>1</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="4">
         <v>54</v>
       </c>
@@ -1779,10 +2000,10 @@
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="18">
         <v>2</v>
       </c>
-      <c r="C9" s="23"/>
+      <c r="C9" s="18"/>
       <c r="D9" s="3">
         <v>35</v>
       </c>
@@ -1803,10 +2024,10 @@
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="18">
         <v>2</v>
       </c>
-      <c r="C10" s="23"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="3">
         <v>25</v>
       </c>
@@ -1846,10 +2067,10 @@
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="18">
         <v>2</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="18"/>
       <c r="D11" s="3">
         <v>27</v>
       </c>
@@ -1870,10 +2091,10 @@
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="18">
         <v>2</v>
       </c>
-      <c r="C12" s="23"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="3">
         <v>26</v>
       </c>
@@ -1894,10 +2115,10 @@
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="18">
         <v>2</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="3">
         <v>31</v>
       </c>
@@ -1918,10 +2139,10 @@
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="19">
         <v>3</v>
       </c>
-      <c r="C14" s="24"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="2">
         <v>33</v>
       </c>
@@ -1942,10 +2163,10 @@
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="19">
         <v>3</v>
       </c>
-      <c r="C15" s="24"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="2">
         <v>30</v>
       </c>
@@ -1966,10 +2187,10 @@
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="19">
         <v>3</v>
       </c>
-      <c r="C16" s="24"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="2">
         <v>40</v>
       </c>
@@ -1990,10 +2211,10 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="17">
         <v>4</v>
       </c>
-      <c r="C17" s="25"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="1">
         <v>14</v>
       </c>
@@ -2014,10 +2235,10 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="17">
         <v>4</v>
       </c>
-      <c r="C18" s="25"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="15">
         <v>28</v>
       </c>
@@ -2038,10 +2259,10 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="25">
+      <c r="B19" s="17">
         <v>4</v>
       </c>
-      <c r="C19" s="25"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="1">
         <v>20</v>
       </c>
@@ -2062,10 +2283,10 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B20" s="17">
         <v>4</v>
       </c>
-      <c r="C20" s="25"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="1">
         <v>21</v>
       </c>
@@ -2086,12 +2307,12 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="17">
         <v>4</v>
       </c>
-      <c r="C21" s="25"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="1">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E21" s="1">
         <v>13</v>
@@ -2110,10 +2331,10 @@
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="25">
+      <c r="B22" s="17">
         <v>4</v>
       </c>
-      <c r="C22" s="25"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="1">
         <v>25</v>
       </c>
@@ -2134,10 +2355,10 @@
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="25">
+      <c r="B23" s="17">
         <v>4</v>
       </c>
-      <c r="C23" s="25"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="1">
         <v>18</v>
       </c>
@@ -2158,10 +2379,10 @@
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="25">
+      <c r="B24" s="17">
         <v>4</v>
       </c>
-      <c r="C24" s="25"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="1">
         <v>16</v>
       </c>
@@ -2182,16 +2403,16 @@
       <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D27" s="8">
         <f>AVERAGE(D2:D24)</f>
-        <v>35.217391304347828</v>
+        <v>34.782608695652172</v>
       </c>
       <c r="E27" s="8">
         <f t="shared" ref="E27:F27" si="1">AVERAGE(E2:E24)</f>
@@ -2203,13 +2424,13 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
@@ -2230,8 +2451,8 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C31" s="9" t="s">
-        <v>1</v>
+      <c r="C31" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="D31" s="10">
         <f>AVERAGE(D2:D8)</f>
@@ -2247,15 +2468,15 @@
       </c>
       <c r="G31" s="10">
         <f>AVERAGE(D17:D24)</f>
-        <v>20.5</v>
+        <v>19.25</v>
       </c>
       <c r="H31" s="10">
         <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C32" s="9" t="s">
-        <v>2</v>
+      <c r="C32" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="D32" s="10">
         <f>AVERAGE(E2:E8)</f>
@@ -2278,8 +2499,8 @@
       </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="9" t="s">
-        <v>3</v>
+      <c r="C33" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="D33" s="10">
         <f>AVERAGE(F2:F8)</f>
@@ -2314,13 +2535,13 @@
       <c r="F35" s="10"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C37" s="11"/>
@@ -2357,7 +2578,10 @@
         <f>COUNTIF(G$17:$G$24,"=OF")</f>
         <v>5</v>
       </c>
-      <c r="H38" s="16"/>
+      <c r="H38" s="16">
+        <f>SUM(D38:G38)/A24</f>
+        <v>0.65217391304347827</v>
+      </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C39" s="11" t="s">
@@ -2379,7 +2603,10 @@
         <f>COUNTIF(G$17:$G$24,"=M")</f>
         <v>2</v>
       </c>
-      <c r="H39" s="16"/>
+      <c r="H39" s="16">
+        <f>SUM(D39:G39)/A24</f>
+        <v>0.30434782608695654</v>
+      </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C40" s="11" t="s">
@@ -2401,7 +2628,10 @@
         <f>COUNTIF(G$17:$G$24,"=FTU")</f>
         <v>1</v>
       </c>
-      <c r="H40" s="16"/>
+      <c r="H40" s="16">
+        <f>SUM(D40:G40)/A24</f>
+        <v>4.3478260869565216E-2</v>
+      </c>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D41" s="9"/>
@@ -2409,13 +2639,13 @@
       <c r="F41" s="9"/>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C43" s="11"/>
@@ -2452,7 +2682,10 @@
         <f>COUNTIF(H$17:$H$24,"=OF")</f>
         <v>0</v>
       </c>
-      <c r="H44" s="16"/>
+      <c r="H44" s="16">
+        <f>SUM(D44:G44)/A24</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C45" s="11" t="s">
@@ -2474,7 +2707,10 @@
         <f>COUNTIF(H$17:$H$24,"=M")</f>
         <v>1</v>
       </c>
-      <c r="H45" s="16"/>
+      <c r="H45" s="16">
+        <f>SUM(D45:G45)/A24</f>
+        <v>4.3478260869565216E-2</v>
+      </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C46" s="11" t="s">
@@ -2496,22 +2732,13 @@
         <f>COUNTIF(H$17:$H$24,"=FTU")</f>
         <v>7</v>
       </c>
-      <c r="H46" s="16"/>
+      <c r="H46" s="16">
+        <f>SUM(D46:G46)/A24</f>
+        <v>0.95652173913043481</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C42:G42"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="C36:G36"/>
@@ -2528,6 +2755,18 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>